<commit_message>
changing template and fix count funciton
</commit_message>
<xml_diff>
--- a/Projects/CCBZA/Data/Template_L&T_November.xlsx
+++ b/Projects/CCBZA/Data/Template_L&T_November.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2510" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2513" uniqueCount="236">
   <si>
     <t xml:space="preserve">Set Name</t>
   </si>
@@ -1157,7 +1157,7 @@
   </sheetPr>
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -1648,7 +1648,7 @@
   </sheetPr>
   <dimension ref="A1:Q76"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="F18" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
@@ -4681,7 +4681,7 @@
   </sheetPr>
   <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
@@ -6091,7 +6091,7 @@
   </sheetPr>
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -6234,7 +6234,7 @@
   </sheetPr>
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -6881,12 +6881,12 @@
   </sheetPr>
   <dimension ref="A1:S99"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K29" activeCellId="0" sqref="K29"/>
+      <selection pane="bottomRight" activeCell="B106" activeCellId="0" sqref="B106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -6902,7 +6902,10 @@
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.6"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="24.9813953488372"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.2744186046512"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="14" min="12" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="28.6744186046512"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.6279069767442"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10851,6 +10854,9 @@
       <c r="O90" s="12" t="s">
         <v>113</v>
       </c>
+      <c r="P90" s="12" t="s">
+        <v>87</v>
+      </c>
       <c r="Q90" s="12" t="s">
         <v>16</v>
       </c>
@@ -10892,6 +10898,9 @@
       <c r="O91" s="12" t="s">
         <v>113</v>
       </c>
+      <c r="P91" s="12" t="s">
+        <v>103</v>
+      </c>
       <c r="Q91" s="12" t="s">
         <v>16</v>
       </c>
@@ -10932,6 +10941,9 @@
       </c>
       <c r="O92" s="12" t="s">
         <v>113</v>
+      </c>
+      <c r="P92" s="12" t="s">
+        <v>133</v>
       </c>
       <c r="Q92" s="12" t="s">
         <v>16</v>

</xml_diff>